<commit_message>
HAJ-1127 , HAJ-1138 : Staff ritual upload
</commit_message>
<xml_diff>
--- a/shj-admin-portal-web/src/main/resources/templates/excel/9/staff-ritual-data.xlsx
+++ b/shj-admin-portal-web/src/main/resources/templates/excel/9/staff-ritual-data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f.messaoudi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\admin-portal\smart-hajj\shj-admin-portal-web\src\main\resources\templates\excel\9\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,34 +26,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>StaffIDNumber  
+    <t>season
+	الموسم الهجرى</t>
+  </si>
+  <si>
+    <t>companyCode
+الشركة</t>
+  </si>
+  <si>
+    <t>IDNumber  
 	رقم الهوية الوطنية / الإقامة</t>
   </si>
   <si>
-    <t>StaffPassportNo
+    <t>PassportNo
 	رقم الجواز</t>
   </si>
   <si>
-    <t>StaffDateOfBirth
+    <t>DateOfBirth
 	تاريخ الميلاد
 DD/MM/YYYY</t>
   </si>
   <si>
-    <t>StaffDateOfBirthHijri
+    <t>DateOfBirthHijri
 	تاريخ الميلاد بالهجري
 YYYYMMDD</t>
   </si>
   <si>
-    <t>season
-	الموسم الهجرى</t>
-  </si>
-  <si>
-    <t xml:space="preserve">staffTypeCode
+    <t xml:space="preserve">RitualTypeCode
 نوع الشعيرة   </t>
-  </si>
-  <si>
-    <t>companyCode
-الشركة</t>
   </si>
 </sst>
 </file>
@@ -432,11 +432,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:H497" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="B3:H497"/>
   <tableColumns count="7">
-    <tableColumn id="2" name="StaffIDNumber  _x000a__x0009_رقم الهوية الوطنية / الإقامة" dataDxfId="6"/>
-    <tableColumn id="3" name="StaffPassportNo_x000a__x0009_رقم الجواز" dataDxfId="5"/>
-    <tableColumn id="7" name="StaffDateOfBirth_x000a__x0009_تاريخ الميلاد_x000a_DD/MM/YYYY" dataDxfId="4"/>
-    <tableColumn id="8" name="StaffDateOfBirthHijri_x000a__x0009_تاريخ الميلاد بالهجري_x000a_YYYYMMDD" dataDxfId="3"/>
-    <tableColumn id="25" name="staffTypeCode_x000a_نوع الشعيرة   " dataDxfId="2"/>
+    <tableColumn id="2" name="IDNumber  _x000a__x0009_رقم الهوية الوطنية / الإقامة" dataDxfId="6"/>
+    <tableColumn id="3" name="PassportNo_x000a__x0009_رقم الجواز" dataDxfId="5"/>
+    <tableColumn id="7" name="DateOfBirth_x000a__x0009_تاريخ الميلاد_x000a_DD/MM/YYYY" dataDxfId="4"/>
+    <tableColumn id="8" name="DateOfBirthHijri_x000a__x0009_تاريخ الميلاد بالهجري_x000a_YYYYMMDD" dataDxfId="3"/>
+    <tableColumn id="25" name="RitualTypeCode_x000a_نوع الشعيرة   " dataDxfId="2"/>
     <tableColumn id="1" name="season_x000a__x0009_الموسم الهجرى" dataDxfId="1"/>
     <tableColumn id="4" name="companyCode_x000a_الشركة" dataDxfId="0"/>
   </tableColumns>
@@ -710,7 +710,7 @@
   <dimension ref="B3:Q1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -736,25 +736,25 @@
   <sheetData>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="H3" s="9" t="s">
         <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.35">
@@ -14285,11 +14285,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
+<XMLData TextToDisplay="%USERNAME%">adhaoui</XMLData>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="RightsWATCHMark">4|ELM-ENG-INT|{00000000-0000-0000-0000-000000000000}</XMLData>
+<XMLData TextToDisplay="%HOSTNAME%">N14946.elm.com.sa</XMLData>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14297,11 +14297,11 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%HOSTNAME%">N14946.elm.com.sa</XMLData>
+<XMLData TextToDisplay="RightsWATCHMark">4|ELM-ENG-INT|{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%USERNAME%">adhaoui</XMLData>
+<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14309,13 +14309,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A04205C-5E94-4530-9C48-4C5414D8E5EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A71EF073-FC9F-4F4A-9348-E778F929AF5B}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1370C946-81E5-4E9E-BD39-1ABD5584D88C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42FEDF57-B554-4217-8153-6D86691A7EEC}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -14327,13 +14327,13 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42FEDF57-B554-4217-8153-6D86691A7EEC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1370C946-81E5-4E9E-BD39-1ABD5584D88C}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A71EF073-FC9F-4F4A-9348-E778F929AF5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A04205C-5E94-4530-9C48-4C5414D8E5EB}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>

</xml_diff>